<commit_message>
Changes to Personal Notes
Added a .txt file with the most important Info for better overview in GitHub
</commit_message>
<xml_diff>
--- a/Documents/LED Current.xlsx
+++ b/Documents/LED Current.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Red</t>
   </si>
@@ -78,7 +78,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -365,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,8 +444,120 @@
         <v>2.2328999999999999</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>104</v>
+      </c>
+      <c r="C9">
+        <f>0.0175*B9+0.4495</f>
+        <v>2.2695000000000003</v>
+      </c>
+      <c r="D9">
+        <f>C9+C10+C11</f>
+        <v>7.3045999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>135</v>
+      </c>
+      <c r="C10">
+        <f>0.0181*B10+0.3587</f>
+        <v>2.8022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>130</v>
+      </c>
+      <c r="C11">
+        <f>0.016*B11+0.1529</f>
+        <v>2.2328999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>255</v>
+      </c>
+      <c r="C16">
+        <f>0.0175*B16+0.4495</f>
+        <v>4.9120000000000008</v>
+      </c>
+      <c r="D16">
+        <f>C16+C17+C18</f>
+        <v>5.4236000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>0.0181*B17+0.3587</f>
+        <v>0.35870000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>0.016*B18+0.1529</f>
+        <v>0.15290000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>4.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>4.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>4.3</formula>
     </cfRule>

</xml_diff>

<commit_message>
New Current cal for white under 4.3 amps
</commit_message>
<xml_diff>
--- a/Documents/LED Current.xlsx
+++ b/Documents/LED Current.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="8">
   <si>
     <t>Red</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Total Current</t>
+  </si>
+  <si>
+    <t>Factpr</t>
+  </si>
+  <si>
+    <t>Def Vals</t>
   </si>
 </sst>
 </file>
@@ -425,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -453,7 +459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -483,7 +489,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -505,7 +511,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -527,7 +533,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -546,21 +552,31 @@
       <c r="I8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>0.5</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1">
-        <v>255</v>
+        <f>N9*$L$8</f>
+        <v>52</v>
       </c>
       <c r="C9">
         <f>0.0175*B9+0.4495</f>
-        <v>4.9120000000000008</v>
+        <v>1.3595000000000002</v>
       </c>
       <c r="D9">
         <f>C9+C10+C11</f>
-        <v>9.9471000000000007</v>
+        <v>4.1328500000000004</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -576,17 +592,21 @@
         <f>SUM(H9:H11)</f>
         <v>12.899999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <v>135</v>
+        <f>N10*$L$8</f>
+        <v>67.5</v>
       </c>
       <c r="C10">
         <f>0.0181*B10+0.3587</f>
-        <v>2.8022</v>
+        <v>1.5804500000000001</v>
       </c>
       <c r="F10" t="s">
         <v>1</v>
@@ -598,17 +618,21 @@
       <c r="H10" s="1">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="1">
-        <v>130</v>
+        <f>N11*$L$8</f>
+        <v>65</v>
       </c>
       <c r="C11">
         <f>0.016*B11+0.1529</f>
-        <v>2.2328999999999999</v>
+        <v>1.1929000000000001</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -620,8 +644,11 @@
       <c r="H11" s="1">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -641,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>

</xml_diff>